<commit_message>
Cleaning of old useless files
</commit_message>
<xml_diff>
--- a/Cohérence des mesures biométriques et de f_nat.xlsx
+++ b/Cohérence des mesures biométriques et de f_nat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crecapet\Documents\Recherche\Modelisation\Dynamic Energy Budget Theory\Salsa_WvsF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vverdon\Documents\MATLAB\Salsa_WvsF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7065"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -403,16 +403,16 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -435,7 +435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,7 +458,7 @@
         <v>0.66620644860950273</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -481,7 +481,7 @@
         <v>0.60325672225218496</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -489,7 +489,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -503,7 +503,7 @@
         <v>0.16259999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -514,7 +514,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -523,7 +523,7 @@
         <v>1.2264150943396226</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>

</xml_diff>